<commit_message>
EPBDS-9207 Method addAll(a[], b, c[]) doesn't work in runtime
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9124_Add_all_method.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9124_Add_all_method.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-9124_Add_all_method\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A8062F-2B13-4E4D-B353-FD8E323E4785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="25875" windowHeight="11820"/>
+    <workbookView xWindow="-32130" yWindow="6360" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
   <si>
     <t>Steps</t>
   </si>
@@ -103,16 +109,23 @@
   </si>
   <si>
     <t>_res_.$Step3[3]</t>
+  </si>
+  <si>
+    <t>_res_.$Step2[3]</t>
+  </si>
+  <si>
+    <t>_res_.$Step2[4]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,14 +149,14 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -170,7 +183,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -179,14 +192,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -224,9 +240,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,9 +275,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,9 +327,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -469,27 +519,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D8:J29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D8:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29:J29"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="24.81640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>0</v>
       </c>
@@ -497,7 +547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>2</v>
       </c>
@@ -505,7 +555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>15</v>
       </c>
@@ -513,7 +563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>19</v>
       </c>
@@ -521,12 +571,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>3</v>
       </c>
@@ -543,7 +593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>3</v>
       </c>
@@ -560,7 +610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>4</v>
       </c>
@@ -577,12 +627,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>3</v>
       </c>
@@ -601,8 +651,14 @@
       <c r="I20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>3</v>
       </c>
@@ -621,8 +677,14 @@
       <c r="I21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
         <v>4</v>
       </c>
@@ -638,16 +700,22 @@
       <c r="H22" t="s">
         <v>10</v>
       </c>
-      <c r="I22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>3</v>
       </c>
@@ -670,7 +738,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
         <v>3</v>
       </c>
@@ -693,7 +761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>4</v>
       </c>
@@ -722,24 +790,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-9316 Method ne(a, b[]) is not found
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9124_Add_all_method.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9124_Add_all_method.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-9124_Add_all_method\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A8062F-2B13-4E4D-B353-FD8E323E4785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A0DDAE-3368-43AC-93B8-86E8C08B1B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32130" yWindow="6360" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="3285" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
   <si>
     <t>Steps</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Step3</t>
   </si>
   <si>
-    <t>Test mySpr mySprTest1</t>
-  </si>
-  <si>
     <t>_res_.$Step2[1]</t>
   </si>
   <si>
@@ -115,17 +112,19 @@
   </si>
   <si>
     <t>_res_.$Step2[4]</t>
+  </si>
+  <si>
+    <t>//Test mySpr mySprTest1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,7 +148,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -523,15 +522,15 @@
   <dimension ref="D8:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="24.81640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.1796875" collapsed="true"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.81640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.7265625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="4:8" x14ac:dyDescent="0.35">
@@ -573,7 +572,7 @@
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.35">
@@ -629,7 +628,7 @@
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.35">
@@ -646,16 +645,16 @@
         <v>17</v>
       </c>
       <c r="H20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" t="s">
         <v>21</v>
       </c>
-      <c r="I20" t="s">
-        <v>22</v>
-      </c>
       <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
         <v>29</v>
-      </c>
-      <c r="K20" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.35">
@@ -672,16 +671,16 @@
         <v>17</v>
       </c>
       <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" t="s">
         <v>21</v>
       </c>
-      <c r="I21" t="s">
-        <v>22</v>
-      </c>
       <c r="J21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" t="s">
         <v>29</v>
-      </c>
-      <c r="K21" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.35">
@@ -712,7 +711,7 @@
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.35">
@@ -726,16 +725,16 @@
         <v>8</v>
       </c>
       <c r="G27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" t="s">
         <v>25</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>26</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>27</v>
-      </c>
-      <c r="J27" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.35">
@@ -749,16 +748,16 @@
         <v>8</v>
       </c>
       <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="s">
         <v>25</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>26</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>27</v>
-      </c>
-      <c r="J28" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
EPBDS-10708 Casts of arrays are wrong in the ternary operation
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9124_Add_all_method.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9124_Add_all_method.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A0DDAE-3368-43AC-93B8-86E8C08B1B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BDE539-AEEE-4EDE-8928-B2ABEA2138A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="3285" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="2410" windowWidth="27500" windowHeight="13310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Steps</t>
   </si>
@@ -108,13 +108,10 @@
     <t>_res_.$Step3[3]</t>
   </si>
   <si>
-    <t>_res_.$Step2[3]</t>
-  </si>
-  <si>
-    <t>_res_.$Step2[4]</t>
-  </si>
-  <si>
     <t>//Test mySpr mySprTest1</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -519,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D8:K29"/>
+  <dimension ref="D8:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +569,7 @@
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.35">
@@ -609,7 +606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>4</v>
       </c>
@@ -626,12 +623,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>3</v>
       </c>
@@ -650,14 +647,8 @@
       <c r="I20" t="s">
         <v>21</v>
       </c>
-      <c r="J20" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>3</v>
       </c>
@@ -676,14 +667,8 @@
       <c r="I21" t="s">
         <v>21</v>
       </c>
-      <c r="J21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
         <v>4</v>
       </c>
@@ -699,22 +684,16 @@
       <c r="H22" t="s">
         <v>10</v>
       </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>2</v>
-      </c>
-      <c r="K22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="I22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>3</v>
       </c>
@@ -737,7 +716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
         <v>3</v>
       </c>
@@ -760,7 +739,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>4</v>
       </c>

</xml_diff>